<commit_message>
Sync updated BOM for multitarget
</commit_message>
<xml_diff>
--- a/hardware/victims/ztex_multivictim/digikey_order_bom.xlsx
+++ b/hardware/victims/ztex_multivictim/digikey_order_bom.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="30" windowWidth="13185" windowHeight="9750" activeTab="2"/>
+    <workbookView xWindow="10800" yWindow="90" windowWidth="13185" windowHeight="9690" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="From Eagle" sheetId="1" r:id="rId1"/>
-    <sheet name="Digikey Upload" sheetId="2" r:id="rId2"/>
-    <sheet name="Digikey Final" sheetId="3" r:id="rId3"/>
+    <sheet name="Digikey Final" sheetId="3" r:id="rId1"/>
+    <sheet name="From Eagle" sheetId="1" r:id="rId2"/>
+    <sheet name="DO NOT USE" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="bom_generic_victim" localSheetId="0">'From Eagle'!$A$1:$I$35</definedName>
+    <definedName name="bom_generic_victim" localSheetId="1">'From Eagle'!$A$1:$I$35</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -827,9 +827,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>'DO NOT USE'!H3*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'DO NOT USE'!I3</f>
+        <v>754-1591-ND</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>'DO NOT USE'!H4*'DO NOT USE'!$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>'DO NOT USE'!I4</f>
+        <v>5003K-ND</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>'DO NOT USE'!H5*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <f>'DO NOT USE'!I5</f>
+        <v>A32701-40-ND</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>'DO NOT USE'!H6*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <f>'DO NOT USE'!I6</f>
+        <v xml:space="preserve">A33184-ND </v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>'DO NOT USE'!H7*'DO NOT USE'!$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="B6" t="str">
+        <f>'DO NOT USE'!I7</f>
+        <v>P100ACT-ND</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="str">
+        <f>'DO NOT USE'!I8</f>
+        <v>1276-1003-1-ND</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>'DO NOT USE'!H10*'DO NOT USE'!$B$9</f>
+        <v>3</v>
+      </c>
+      <c r="B9" t="str">
+        <f>'DO NOT USE'!I10</f>
+        <v>445-1311-1-ND</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>'DO NOT USE'!H11*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <f>'DO NOT USE'!I11</f>
+        <v>1276-1078-1-ND</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>'DO NOT USE'!H13*'DO NOT USE'!$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <f>'DO NOT USE'!I13</f>
+        <v xml:space="preserve">445-1321-1-ND </v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>'DO NOT USE'!H14*'DO NOT USE'!$B$9</f>
+        <v>3</v>
+      </c>
+      <c r="B13" t="str">
+        <f>'DO NOT USE'!I14</f>
+        <v>1276-1026-1-ND</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>'DO NOT USE'!H15*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B14" t="str">
+        <f>'DO NOT USE'!I15</f>
+        <v xml:space="preserve"> A102197CT-ND</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>'DO NOT USE'!H16*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B15" t="str">
+        <f>'DO NOT USE'!I16</f>
+        <v>P220ACT-ND</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>'DO NOT USE'!H17*'DO NOT USE'!$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="B16" t="str">
+        <f>'DO NOT USE'!I17</f>
+        <v xml:space="preserve">493-6024-ND </v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>'DO NOT USE'!H18*'DO NOT USE'!$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="B17" t="str">
+        <f>'DO NOT USE'!I18</f>
+        <v>1276-1999-1-ND</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>'DO NOT USE'!H19*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B18" t="str">
+        <f>'DO NOT USE'!I19</f>
+        <v xml:space="preserve">1276-1074-1-ND </v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>'DO NOT USE'!H20*'DO NOT USE'!$B$9</f>
+        <v>6</v>
+      </c>
+      <c r="B19" t="str">
+        <f>'DO NOT USE'!I20</f>
+        <v>541-49.9CCT-ND</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>'DO NOT USE'!H21*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B20" t="str">
+        <f>'DO NOT USE'!I21</f>
+        <v xml:space="preserve"> P4.7ACT-ND </v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>'DO NOT USE'!H22*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B21" t="str">
+        <f>'DO NOT USE'!I22</f>
+        <v>ATMEGA328P-PU-ND</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>'DO NOT USE'!H23*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B22" t="str">
+        <f>'DO NOT USE'!I23</f>
+        <v>CTX325LVCT-ND</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>'DO NOT USE'!H24*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B23" t="str">
+        <f>'DO NOT USE'!I24</f>
+        <v>CTX929LVCT-ND</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>'DO NOT USE'!H25*'DO NOT USE'!$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="B24" t="str">
+        <f>'DO NOT USE'!I25</f>
+        <v>568-6208-1-ND</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>'DO NOT USE'!H26*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B25" t="str">
+        <f>'DO NOT USE'!I26</f>
+        <v>A100210-ND</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>'DO NOT USE'!H27*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B26" t="str">
+        <f>'DO NOT USE'!I27</f>
+        <v>ATXMEGA16A4-AU-ND</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>'DO NOT USE'!H28*'DO NOT USE'!$B$9</f>
+        <v>25</v>
+      </c>
+      <c r="B27" t="str">
+        <f>'DO NOT USE'!I28</f>
+        <v>S9337-ND</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>'DO NOT USE'!H29*'DO NOT USE'!$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="B28" t="str">
+        <f>'DO NOT USE'!I29</f>
+        <v>609-3530-ND</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1538,7 +1810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J29"/>
   <sheetViews>
@@ -1817,276 +2089,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>'Digikey Upload'!H3*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f>'Digikey Upload'!I3</f>
-        <v>754-1591-ND</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>'Digikey Upload'!H4*'Digikey Upload'!$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f>'Digikey Upload'!I4</f>
-        <v>5003K-ND</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>'Digikey Upload'!H5*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <f>'Digikey Upload'!I5</f>
-        <v>A32701-40-ND</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>'Digikey Upload'!H6*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B5" t="str">
-        <f>'Digikey Upload'!I6</f>
-        <v xml:space="preserve">A33184-ND </v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>'Digikey Upload'!H7*'Digikey Upload'!$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="B6" t="str">
-        <f>'Digikey Upload'!I7</f>
-        <v>P100ACT-ND</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="str">
-        <f>'Digikey Upload'!I8</f>
-        <v>1276-1003-1-ND</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>'Digikey Upload'!H10*'Digikey Upload'!$B$9</f>
-        <v>3</v>
-      </c>
-      <c r="B9" t="str">
-        <f>'Digikey Upload'!I10</f>
-        <v>445-1311-1-ND</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>'Digikey Upload'!H11*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B10" t="str">
-        <f>'Digikey Upload'!I11</f>
-        <v>1276-1078-1-ND</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>'Digikey Upload'!H13*'Digikey Upload'!$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="B12" t="str">
-        <f>'Digikey Upload'!I13</f>
-        <v xml:space="preserve">445-1321-1-ND </v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>'Digikey Upload'!H14*'Digikey Upload'!$B$9</f>
-        <v>3</v>
-      </c>
-      <c r="B13" t="str">
-        <f>'Digikey Upload'!I14</f>
-        <v>1276-1026-1-ND</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>'Digikey Upload'!H15*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B14" t="str">
-        <f>'Digikey Upload'!I15</f>
-        <v xml:space="preserve"> A102197CT-ND</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>'Digikey Upload'!H16*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B15" t="str">
-        <f>'Digikey Upload'!I16</f>
-        <v>P220ACT-ND</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>'Digikey Upload'!H17*'Digikey Upload'!$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="B16" t="str">
-        <f>'Digikey Upload'!I17</f>
-        <v xml:space="preserve">493-6024-ND </v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>'Digikey Upload'!H18*'Digikey Upload'!$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="B17" t="str">
-        <f>'Digikey Upload'!I18</f>
-        <v>1276-1999-1-ND</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>'Digikey Upload'!H19*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B18" t="str">
-        <f>'Digikey Upload'!I19</f>
-        <v xml:space="preserve">1276-1074-1-ND </v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>'Digikey Upload'!H20*'Digikey Upload'!$B$9</f>
-        <v>6</v>
-      </c>
-      <c r="B19" t="str">
-        <f>'Digikey Upload'!I20</f>
-        <v>541-49.9CCT-ND</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f>'Digikey Upload'!H21*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B20" t="str">
-        <f>'Digikey Upload'!I21</f>
-        <v xml:space="preserve"> P4.7ACT-ND </v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f>'Digikey Upload'!H22*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B21" t="str">
-        <f>'Digikey Upload'!I22</f>
-        <v>ATMEGA328P-PU-ND</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f>'Digikey Upload'!H23*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B22" t="str">
-        <f>'Digikey Upload'!I23</f>
-        <v>CTX325LVCT-ND</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f>'Digikey Upload'!H24*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B23" t="str">
-        <f>'Digikey Upload'!I24</f>
-        <v>CTX929LVCT-ND</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f>'Digikey Upload'!H25*'Digikey Upload'!$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="B24" t="str">
-        <f>'Digikey Upload'!I25</f>
-        <v>568-6208-1-ND</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f>'Digikey Upload'!H26*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B25" t="str">
-        <f>'Digikey Upload'!I26</f>
-        <v>A100210-ND</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f>'Digikey Upload'!H27*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B26" t="str">
-        <f>'Digikey Upload'!I27</f>
-        <v>ATXMEGA16A4-AU-ND</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f>'Digikey Upload'!H28*'Digikey Upload'!$B$9</f>
-        <v>25</v>
-      </c>
-      <c r="B27" t="str">
-        <f>'Digikey Upload'!I28</f>
-        <v>S9337-ND</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f>'Digikey Upload'!H29*'Digikey Upload'!$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="B28" t="str">
-        <f>'Digikey Upload'!I29</f>
-        <v>609-3530-ND</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>